<commit_message>
fixed time problem and wrote something on sop
</commit_message>
<xml_diff>
--- a/physics/fjederkonstant.xlsx
+++ b/physics/fjederkonstant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ktsdk-my.sharepoint.com/personal/nick473a_edu_nextkbh_dk/Documents/node projects/SOP-project/physics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{65D100B1-2E2F-45BF-8A0D-C71902AC9EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A13DF1B8-CF53-4527-A2EB-7CE47863FFEF}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="8_{65D100B1-2E2F-45BF-8A0D-C71902AC9EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABBBD5C1-1377-41E8-BBB8-1063D27C9FE7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D01E7BE3-D6F6-4378-BAE4-53E291F428CD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>fjeder mappings ved 13.5 cm</t>
   </si>
@@ -52,6 +52,57 @@
   </si>
   <si>
     <t>converted</t>
+  </si>
+  <si>
+    <t>bar længde</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>bar vægt</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>weight weight</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>camera angle</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>weight height</t>
+  </si>
+  <si>
+    <t>weight r</t>
+  </si>
+  <si>
+    <t>disc r</t>
+  </si>
+  <si>
+    <t>disc weight</t>
+  </si>
+  <si>
+    <t>ball weight</t>
+  </si>
+  <si>
+    <t>ball diameter</t>
+  </si>
+  <si>
+    <t>ring weight</t>
+  </si>
+  <si>
+    <t>ring dia</t>
   </si>
 </sst>
 </file>
@@ -3453,20 +3504,130 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09927A40-3AF2-4E28-9E3B-6CBD43151094}">
-  <dimension ref="A3:F25"/>
+  <dimension ref="A2:AG25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AH2" sqref="AH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V2" t="s">
+        <v>17</v>
+      </c>
+      <c r="X2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
+      <c r="J3">
+        <v>0.6</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3">
+        <v>0.128</v>
+      </c>
+      <c r="M3" t="s">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="O3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3">
+        <v>4</v>
+      </c>
+      <c r="S3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3">
+        <v>1.5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>7</v>
+      </c>
+      <c r="V3">
+        <v>10.8</v>
+      </c>
+      <c r="W3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X3">
+        <v>270</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3">
+        <v>860</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AB3">
+        <v>14</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD3">
+        <v>351</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF3">
+        <v>10</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3477,7 +3638,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -3491,7 +3652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>15</v>
       </c>
@@ -3505,7 +3666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>35</v>
       </c>
@@ -3527,7 +3688,7 @@
         <v>-3.9149999999999997E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>45</v>
       </c>
@@ -3549,7 +3710,7 @@
         <v>-3.1050000000000005E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>55</v>
       </c>
@@ -3571,7 +3732,7 @@
         <v>-2.7000000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>65</v>
       </c>
@@ -3593,7 +3754,7 @@
         <v>-2.3625E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>75</v>
       </c>
@@ -3615,7 +3776,7 @@
         <v>-1.917E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>85</v>
       </c>
@@ -3637,7 +3798,7 @@
         <v>-1.6064999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>95</v>
       </c>
@@ -3659,7 +3820,7 @@
         <v>-1.2015E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>105</v>
       </c>
@@ -3681,7 +3842,7 @@
         <v>-9.1800000000000007E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>115</v>
       </c>
@@ -3697,7 +3858,7 @@
         <v>2.7000000000000001E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
it is complete :relieved:
</commit_message>
<xml_diff>
--- a/physics/fjederkonstant.xlsx
+++ b/physics/fjederkonstant.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="76" documentId="8_{65D100B1-2E2F-45BF-8A0D-C71902AC9EDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{20481493-1C89-4441-9F69-DF886E1887DF}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="7605" windowWidth="29040" windowHeight="15840" xr2:uid="{D01E7BE3-D6F6-4378-BAE4-53E291F428CD}"/>
+    <workbookView minimized="1" xWindow="38745" yWindow="8055" windowWidth="28800" windowHeight="15435" xr2:uid="{D01E7BE3-D6F6-4378-BAE4-53E291F428CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3546,7 +3546,7 @@
   <dimension ref="A2:AG25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>